<commit_message>
Updated my Sprint Backlog hours
</commit_message>
<xml_diff>
--- a/documentation/HyreDefyer Sprint Backlog Burndown.xlsx
+++ b/documentation/HyreDefyer Sprint Backlog Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28627"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcorley\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kynda\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2558366-92C3-42E7-9EC0-9C4656465917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EF4B39-37F8-4D7F-8F8E-23467CCAA7E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -213,7 +213,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,14 +424,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -550,16 +550,16 @@
                   <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45.5</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1603,42 +1603,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="85.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="85.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="20" t="s">
+      <c r="C1" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
       <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1836,8 +1836,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1">
-      <c r="A11" s="22" t="s">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -1847,19 +1847,19 @@
         <v>8</v>
       </c>
       <c r="D11" s="6">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E11" s="6">
-        <v>8</v>
+        <v>0.5</v>
       </c>
       <c r="F11" s="6">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G11" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -1893,19 +1893,19 @@
         <v>3</v>
       </c>
       <c r="D13" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E13" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G13" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>17</v>
       </c>
@@ -1916,19 +1916,19 @@
         <v>3</v>
       </c>
       <c r="D14" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E14" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F14" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G14" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>24</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>24</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>8</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>24</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>32</v>
       </c>
@@ -2122,44 +2122,44 @@
       </c>
       <c r="D23" s="2">
         <f>SUM(D3:D22)</f>
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E23" s="2">
         <f>SUM(E3:E22)</f>
-        <v>45.5</v>
+        <v>34</v>
       </c>
       <c r="F23" s="2">
         <f>SUM(F3:F22)</f>
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G23" s="2">
         <f>SUM(G3:G22)</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="21" t="s">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="22" t="s">
         <v>2</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
       <c r="D26" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>8</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>8</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>8</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>8</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>8</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>8</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>24</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>24</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>19</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>19</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>19</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>19</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>46</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>46</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>8</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>8</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>46</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>8</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>8</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>46</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>46</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>8</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="2:3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" s="3" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Updated Sprint Backlog and Burndown
Updated the documentation for sprint backlog and burndown.
</commit_message>
<xml_diff>
--- a/documentation/HyreDefyer Sprint Backlog Burndown.xlsx
+++ b/documentation/HyreDefyer Sprint Backlog Burndown.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28627"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kynda\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://westga365-my.sharepoint.com/personal/jb00645_my_westga_edu/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EF4B39-37F8-4D7F-8F8E-23467CCAA7E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEF9D4C3-5717-449E-8F0B-9CEC691C9C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="65">
   <si>
     <t>Task Manager / Dev</t>
   </si>
@@ -137,6 +137,9 @@
     <t>Estimate Totals</t>
   </si>
   <si>
+    <t>Hours Worked</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rounded to </t>
   </si>
   <si>
@@ -207,13 +210,34 @@
   </si>
   <si>
     <t xml:space="preserve">Implmented and Binded All of the Category and Category Pull Down and Fixed several errors. </t>
+  </si>
+  <si>
+    <t>Added Functionality to DM page you can now see other users to chat and send messages</t>
+  </si>
+  <si>
+    <t>Implement ability to efficiently switch between views</t>
+  </si>
+  <si>
+    <t>Implemented SignInViewModel</t>
+  </si>
+  <si>
+    <t>Implemented UI Binding for SignInView and SignInViewModel</t>
+  </si>
+  <si>
+    <t>Implemented and Tested Sign Out method</t>
+  </si>
+  <si>
+    <t>Added functionality to header buttons Home and DM</t>
+  </si>
+  <si>
+    <t>Binded functionality to Sign Out buttons</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -395,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -425,6 +449,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -550,16 +577,16 @@
                   <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.5</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1601,44 +1628,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="85.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="85.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="21" t="s">
+      <c r="C1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
       <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1652,7 +1679,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -1675,7 +1702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1698,7 +1725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1721,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1744,7 +1771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
@@ -1767,7 +1794,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
@@ -1790,7 +1817,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -1813,7 +1840,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1836,7 +1863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15" customHeight="1">
       <c r="A11" s="20" t="s">
         <v>17</v>
       </c>
@@ -1847,19 +1874,19 @@
         <v>8</v>
       </c>
       <c r="D11" s="6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E11" s="6">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="F11" s="6">
         <v>2</v>
       </c>
       <c r="G11" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
@@ -1882,7 +1909,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -1893,19 +1920,19 @@
         <v>3</v>
       </c>
       <c r="D13" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E13" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="6">
         <v>1</v>
       </c>
       <c r="G13" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="5" t="s">
         <v>17</v>
       </c>
@@ -1916,19 +1943,19 @@
         <v>3</v>
       </c>
       <c r="D14" s="6">
+        <v>3</v>
+      </c>
+      <c r="E14" s="6">
+        <v>3</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6">
         <v>0</v>
       </c>
-      <c r="E14" s="6">
-        <v>0</v>
-      </c>
-      <c r="F14" s="6">
-        <v>2</v>
-      </c>
-      <c r="G14" s="6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
@@ -1951,7 +1978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16" s="5" t="s">
         <v>24</v>
       </c>
@@ -1974,7 +2001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -1997,7 +2024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7">
       <c r="A18" s="5" t="s">
         <v>24</v>
       </c>
@@ -2020,7 +2047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7">
       <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
@@ -2043,7 +2070,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7">
       <c r="A20" s="5" t="s">
         <v>8</v>
       </c>
@@ -2066,7 +2093,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7">
       <c r="A21" s="5" t="s">
         <v>24</v>
       </c>
@@ -2089,7 +2116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -2112,7 +2139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="B23" s="3" t="s">
         <v>32</v>
       </c>
@@ -2122,121 +2149,121 @@
       </c>
       <c r="D23" s="2">
         <f>SUM(D3:D22)</f>
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E23" s="2">
         <f>SUM(E3:E22)</f>
-        <v>34</v>
+        <v>38.5</v>
       </c>
       <c r="F23" s="2">
         <f>SUM(F3:F22)</f>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G23" s="2">
         <f>SUM(G3:G22)</f>
-        <v>19.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="22" t="s">
-        <v>2</v>
+      <c r="C25" s="23" t="s">
+        <v>33</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="23"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
       <c r="D26" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C27" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7">
       <c r="A28" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7">
       <c r="A29" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7">
       <c r="A30" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C30" s="1">
         <v>1.5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7">
       <c r="A31" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7">
       <c r="A32" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C32" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5">
       <c r="A33" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C33" s="1">
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5">
       <c r="A34" s="5" t="s">
         <v>24</v>
       </c>
@@ -2247,169 +2274,248 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5">
       <c r="A35" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C35" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5">
       <c r="A36" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C36" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5">
       <c r="A37" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C37" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5">
       <c r="A38" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C38" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5">
       <c r="A39" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C39" s="1">
         <v>1.5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5">
       <c r="A40" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C40" s="1">
         <v>3.5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5">
       <c r="A41" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C41" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5">
       <c r="A42" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C42" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5">
       <c r="A43" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C43" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5">
       <c r="A44" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C44" s="1">
         <v>3.5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5">
       <c r="A45" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C45" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="15">
       <c r="A46" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C46" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E46" s="21"/>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C47" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5">
       <c r="A48" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C48" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B49" s="3" t="s">
+    <row r="49" spans="1:3">
+      <c r="A49" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C51" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15">
+      <c r="A55" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="B56" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C49" s="2">
-        <f>SUM(C27:C48)</f>
-        <v>47</v>
-      </c>
-    </row>
+      <c r="C56" s="2">
+        <f>SUM(C27:C55)</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="D1:G1"/>

</xml_diff>